<commit_message>
Published state of ETDataset on September 2022
</commit_message>
<xml_diff>
--- a/eu_datasets/power_plants/20220609_EU_power_plants.xlsx
+++ b/eu_datasets/power_plants/20220609_EU_power_plants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/etdataset/eu_datasets/power_plants/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathijsbijkerk/Projects/etdataset/eu_datasets/power_plants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9141729-DC0D-0943-B02C-CDA11E63B410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D5C545-5AAB-484C-B773-7777C740AA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54400" yWindow="-18300" windowWidth="25600" windowHeight="28300" activeTab="4" xr2:uid="{66A93571-7039-6645-A132-175564A037D7}"/>
+    <workbookView xWindow="32000" yWindow="500" windowWidth="32000" windowHeight="17180" firstSheet="2" activeTab="2" xr2:uid="{66A93571-7039-6645-A132-175564A037D7}"/>
   </bookViews>
   <sheets>
     <sheet name="introduction" sheetId="12" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="346">
   <si>
     <t>Coal pulverized</t>
   </si>
@@ -16825,8 +16825,8 @@
   </sheetPr>
   <dimension ref="A1:AE34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AD3" sqref="AD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17053,7 +17053,7 @@
       </c>
       <c r="AD3" s="11">
         <f>INDEX('FLH renewables ninja'!$C:$C,MATCH('calculation renewable pp'!AD$2,'FLH renewables ninja'!$A:$A,0),1)</f>
-        <v>1556.84</v>
+        <v>1217.9682842756854</v>
       </c>
       <c r="AE3" s="11">
         <f>INDEX('FLH renewables ninja'!$C:$C,MATCH('calculation renewable pp'!AE$2,'FLH renewables ninja'!$A:$A,0),1)</f>
@@ -17177,7 +17177,7 @@
       </c>
       <c r="AD4" s="11">
         <f>INDEX('FLH renewables ninja'!$C:$C,MATCH('calculation renewable pp'!AD$2,'FLH renewables ninja'!$A:$A,0),1)</f>
-        <v>1556.84</v>
+        <v>1217.9682842756854</v>
       </c>
       <c r="AE4" s="11">
         <f>INDEX('FLH renewables ninja'!$C:$C,MATCH('calculation renewable pp'!AE$2,'FLH renewables ninja'!$A:$A,0),1)</f>
@@ -17301,7 +17301,7 @@
       </c>
       <c r="AD5" s="11">
         <f>INDEX('FLH renewables ninja'!$C:$C,MATCH('calculation renewable pp'!AD$2,'FLH renewables ninja'!$A:$A,0),1)</f>
-        <v>1556.84</v>
+        <v>1217.9682842756854</v>
       </c>
       <c r="AE5" s="11">
         <f>INDEX('FLH renewables ninja'!$C:$C,MATCH('calculation renewable pp'!AE$2,'FLH renewables ninja'!$A:$A,0),1)</f>
@@ -26933,7 +26933,7 @@
   </sheetPr>
   <dimension ref="A1:AT81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -41170,7 +41170,7 @@
   <dimension ref="A1:O165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -42339,8 +42339,9 @@
       <c r="B29" s="44" t="s">
         <v>340</v>
       </c>
-      <c r="C29">
-        <v>1556.84</v>
+      <c r="C29" s="46">
+        <f>O29*M$7</f>
+        <v>1217.9682842756854</v>
       </c>
       <c r="D29" s="47" t="s">
         <v>196</v>
@@ -42362,6 +42363,12 @@
       </c>
       <c r="J29" s="47" t="s">
         <v>199</v>
+      </c>
+      <c r="N29" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="O29" s="46">
+        <v>1556.836</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -42384,63 +42391,69 @@
         <v>2951.1932144574498</v>
       </c>
     </row>
-    <row r="38" spans="5:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="46"/>
+    </row>
+    <row r="34" spans="3:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="46"/>
+    </row>
+    <row r="38" spans="3:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E38" s="49"/>
       <c r="F38" s="49"/>
       <c r="G38" s="49"/>
       <c r="H38" s="49"/>
     </row>
-    <row r="39" spans="5:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E39" s="49"/>
       <c r="F39" s="49"/>
       <c r="G39" s="49"/>
       <c r="H39" s="49"/>
     </row>
-    <row r="40" spans="5:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G40" s="49"/>
       <c r="H40" s="49"/>
     </row>
-    <row r="41" spans="5:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E41" s="49"/>
       <c r="F41" s="49"/>
       <c r="G41" s="49"/>
       <c r="H41" s="49"/>
     </row>
-    <row r="42" spans="5:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E42" s="49"/>
       <c r="F42" s="49"/>
       <c r="G42" s="49"/>
       <c r="H42" s="49"/>
     </row>
-    <row r="43" spans="5:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E43" s="49"/>
       <c r="F43" s="49"/>
       <c r="G43" s="49"/>
       <c r="H43" s="49"/>
     </row>
-    <row r="44" spans="5:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E44" s="49"/>
       <c r="F44" s="49"/>
       <c r="G44" s="49"/>
       <c r="H44" s="49"/>
     </row>
-    <row r="45" spans="5:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G45" s="49"/>
       <c r="H45" s="49"/>
     </row>
-    <row r="46" spans="5:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E46" s="49"/>
       <c r="F46" s="49"/>
       <c r="G46" s="49"/>
       <c r="H46" s="49"/>
     </row>
-    <row r="47" spans="5:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E47" s="49"/>
       <c r="F47" s="49"/>
       <c r="G47" s="49"/>
       <c r="H47" s="49"/>
     </row>
-    <row r="48" spans="5:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E48" s="49"/>
       <c r="F48" s="49"/>
       <c r="G48" s="49"/>

</xml_diff>